<commit_message>
Make pseudocode for test case tp_01
</commit_message>
<xml_diff>
--- a/test_case/Doku_task.xlsx
+++ b/test_case/Doku_task.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t>Test ID</t>
   </si>
@@ -140,6 +140,20 @@
   </si>
   <si>
     <t>Transaksi gagal dan muncul pop up error messages "Transaction Failed. Transfer process has exceeded the maximum number of transfers in a day "</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Start
+Initialize Total Transfer = Input value total transfer
+Initialize Limit Balance = 10 million
+Read Balance Total = Value balance now
+Input Total Transfer
+   IF Total Transfer + Balance Total &lt;= Limit Balance
+        Print "Transaction Success"
+   ELSE
+        Print "Transaction Failed. Maximum balance is Limit Balance"
+   ENDIF
+End
+</t>
   </si>
 </sst>
 </file>
@@ -278,7 +292,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -346,6 +360,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -633,7 +650,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F7"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -666,7 +683,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="142.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="156" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>6</v>
       </c>
@@ -682,7 +699,9 @@
       <c r="E2" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="12"/>
+      <c r="F2" s="24" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="3" spans="1:6" ht="145.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">

</xml_diff>

<commit_message>
Add pseudocode for test case tp_02
</commit_message>
<xml_diff>
--- a/test_case/Doku_task.xlsx
+++ b/test_case/Doku_task.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
   <si>
     <t>Test ID</t>
   </si>
@@ -151,6 +151,20 @@
         Print "Transaction Success"
    ELSE
         Print "Transaction Failed. Maximum balance is Limit Balance"
+   ENDIF
+End
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Start
+Initialize Total Transfer = Input value total transfer
+Initialize Minimum Transfer = 10,000
+Read Balance Total = Value balance now
+Input Total Transfer
+   IF Total Transfer &gt; Minimum Transfer
+        Print "Transaction Success"
+   ELSE
+        Print "Transaction Failed. Minimum total transfer is Minimum Transfer"
    ENDIF
 End
 </t>
@@ -292,7 +306,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -343,6 +357,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -362,7 +379,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -650,7 +667,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -687,7 +704,7 @@
       <c r="A2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="19" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="9" t="s">
@@ -699,7 +716,7 @@
       <c r="E2" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="24" t="s">
+      <c r="F2" s="18" t="s">
         <v>27</v>
       </c>
     </row>
@@ -707,7 +724,7 @@
       <c r="A3" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="19"/>
+      <c r="B3" s="20"/>
       <c r="C3" s="13" t="s">
         <v>11</v>
       </c>
@@ -717,13 +734,15 @@
       <c r="E3" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="12"/>
+      <c r="F3" s="25" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="4" spans="1:6" ht="156.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="20"/>
+      <c r="B4" s="21"/>
       <c r="C4" s="14" t="s">
         <v>14</v>
       </c>
@@ -739,7 +758,7 @@
       <c r="A5" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="22" t="s">
         <v>16</v>
       </c>
       <c r="C5" s="9" t="s">
@@ -757,7 +776,7 @@
       <c r="A6" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="22"/>
+      <c r="B6" s="23"/>
       <c r="C6" s="16" t="s">
         <v>11</v>
       </c>
@@ -773,7 +792,7 @@
       <c r="A7" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="23"/>
+      <c r="B7" s="24"/>
       <c r="C7" s="14" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
Add pseudocode for test case tp_04
</commit_message>
<xml_diff>
--- a/test_case/Doku_task.xlsx
+++ b/test_case/Doku_task.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
   <si>
     <t>Test ID</t>
   </si>
@@ -179,6 +179,18 @@
         Print "Transaction Success"
    ELSE
         Print "Transaction Failed. Transfer process has exceeded the maximum number of transfers in a day "
+   ENDIF
+End
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Start
+Initialize Total Transfer = Input value total transfer
+Initialize Limit Balance = 10 million
+Read Balance Total = Value balance now
+Input Total Transfer
+   IF Total Transfer + Balance Total &gt; Limit Balance
+        Print "Transaction Failed. Maximum balance is Limit Balance"
    ENDIF
 End
 </t>
@@ -359,9 +371,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -391,6 +400,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -677,8 +689,8 @@
   </sheetPr>
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -715,7 +727,7 @@
       <c r="A2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="18" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="9" t="s">
@@ -727,7 +739,7 @@
       <c r="E2" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="16" t="s">
         <v>27</v>
       </c>
     </row>
@@ -735,7 +747,7 @@
       <c r="A3" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="20"/>
+      <c r="B3" s="19"/>
       <c r="C3" s="12" t="s">
         <v>11</v>
       </c>
@@ -745,7 +757,7 @@
       <c r="E3" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="18" t="s">
+      <c r="F3" s="17" t="s">
         <v>28</v>
       </c>
     </row>
@@ -753,7 +765,7 @@
       <c r="A4" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="21"/>
+      <c r="B4" s="20"/>
       <c r="C4" s="13" t="s">
         <v>14</v>
       </c>
@@ -763,7 +775,7 @@
       <c r="E4" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="18" t="s">
+      <c r="F4" s="17" t="s">
         <v>29</v>
       </c>
     </row>
@@ -771,7 +783,7 @@
       <c r="A5" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="21" t="s">
         <v>16</v>
       </c>
       <c r="C5" s="9" t="s">
@@ -783,14 +795,16 @@
       <c r="E5" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="14"/>
+      <c r="F5" s="24" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="6" spans="1:6" ht="132" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="15" t="s">
+      <c r="B6" s="22"/>
+      <c r="C6" s="14" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -799,13 +813,13 @@
       <c r="E6" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="16"/>
+      <c r="F6" s="15"/>
     </row>
     <row r="7" spans="1:6" ht="139.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="24"/>
+      <c r="B7" s="23"/>
       <c r="C7" s="13" t="s">
         <v>19</v>
       </c>
@@ -815,7 +829,7 @@
       <c r="E7" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="16"/>
+      <c r="F7" s="15"/>
     </row>
     <row r="24" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C24" s="2"/>

</xml_diff>

<commit_message>
Add pseudocode for test case tp_05
</commit_message>
<xml_diff>
--- a/test_case/Doku_task.xlsx
+++ b/test_case/Doku_task.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
   <si>
     <t>Test ID</t>
   </si>
@@ -191,6 +191,18 @@
 Input Total Transfer
    IF Total Transfer + Balance Total &gt; Limit Balance
         Print "Transaction Failed. Maximum balance is Limit Balance"
+   ENDIF
+End
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Start
+Initialize Total Transfer = Input value total transfer
+Initialize Minimum Transfer = 10,000
+Read Balance Total = Value balance now
+Input Total Transfer
+   IF Total Transfer &lt; Minimum Transfer
+        Print "Transaction Failed. Minimum total transfer is Minimum Transfer"
    ENDIF
 End
 </t>
@@ -383,6 +395,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -400,9 +415,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -727,7 +739,7 @@
       <c r="A2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="19" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="9" t="s">
@@ -747,7 +759,7 @@
       <c r="A3" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="19"/>
+      <c r="B3" s="20"/>
       <c r="C3" s="12" t="s">
         <v>11</v>
       </c>
@@ -765,7 +777,7 @@
       <c r="A4" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="20"/>
+      <c r="B4" s="21"/>
       <c r="C4" s="13" t="s">
         <v>14</v>
       </c>
@@ -783,7 +795,7 @@
       <c r="A5" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="22" t="s">
         <v>16</v>
       </c>
       <c r="C5" s="9" t="s">
@@ -795,7 +807,7 @@
       <c r="E5" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="24" t="s">
+      <c r="F5" s="18" t="s">
         <v>30</v>
       </c>
     </row>
@@ -803,7 +815,7 @@
       <c r="A6" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="22"/>
+      <c r="B6" s="23"/>
       <c r="C6" s="14" t="s">
         <v>11</v>
       </c>
@@ -813,13 +825,15 @@
       <c r="E6" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="15"/>
+      <c r="F6" s="15" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="7" spans="1:6" ht="139.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="23"/>
+      <c r="B7" s="24"/>
       <c r="C7" s="13" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
Add pseudocode for test case tp_06
</commit_message>
<xml_diff>
--- a/test_case/Doku_task.xlsx
+++ b/test_case/Doku_task.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
   <si>
     <t>Test ID</t>
   </si>
@@ -203,6 +203,18 @@
 Input Total Transfer
    IF Total Transfer &lt; Minimum Transfer
         Print "Transaction Failed. Minimum total transfer is Minimum Transfer"
+   ENDIF
+End
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Start
+Initialize Total Transfer = Input value total transfer
+Initialize Maximum Transfer = 5 million
+Read Time = Time now/ 24 hours
+Input Total Transfer
+   IF Total Transfer &gt; Maximum Transfer for Time
+        Print "Transaction Failed. Transfer process has exceeded the maximum number of transfers in a day "
    ENDIF
 End
 </t>
@@ -701,8 +713,8 @@
   </sheetPr>
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -843,7 +855,9 @@
       <c r="E7" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="15"/>
+      <c r="F7" s="15" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="24" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C24" s="2"/>

</xml_diff>